<commit_message>
Add UI and game loop
</commit_message>
<xml_diff>
--- a/resources/LevelEditor.xlsx
+++ b/resources/LevelEditor.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="7">
   <si>
     <t>Normal</t>
   </si>
@@ -94,7 +94,77 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="15">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -433,15 +503,13 @@
   <dimension ref="A1:R32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P32" sqref="P32"/>
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:18" ht="15" customHeight="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -456,9 +524,7 @@
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
-      <c r="P1" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="P1" s="1"/>
       <c r="Q1" t="s">
         <v>5</v>
       </c>
@@ -540,14 +606,30 @@
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
+      <c r="E5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
@@ -564,14 +646,30 @@
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
+      <c r="E6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
@@ -588,14 +686,30 @@
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
+      <c r="E7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
@@ -612,14 +726,30 @@
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
+      <c r="E8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
@@ -633,14 +763,30 @@
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
+      <c r="E9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
@@ -654,14 +800,30 @@
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
+      <c r="E10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
@@ -675,14 +837,30 @@
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
+      <c r="E11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
@@ -696,14 +874,30 @@
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
+      <c r="E12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
@@ -783,21 +977,11 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-      <c r="H16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="L16" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
@@ -1122,9 +1306,7 @@
       </c>
     </row>
     <row r="32" spans="1:17" ht="15" customHeight="1">
-      <c r="A32" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
@@ -1139,28 +1321,26 @@
       <c r="M32" s="1"/>
       <c r="N32" s="1"/>
       <c r="O32" s="1"/>
-      <c r="P32" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="P32" s="1"/>
       <c r="Q32" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:P32">
-    <cfRule type="cellIs" dxfId="4" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="11" operator="equal">
       <formula>$R$7</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="12" operator="equal">
       <formula>$R$6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="13" operator="equal">
       <formula>$R$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="14" operator="equal">
       <formula>$R$4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="15" operator="equal">
       <formula>$R$3</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Add more UI and end game
</commit_message>
<xml_diff>
--- a/resources/LevelEditor.xlsx
+++ b/resources/LevelEditor.xlsx
@@ -16,18 +16,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="5">
   <si>
     <t>Normal</t>
   </si>
   <si>
     <t>Explosive</t>
-  </si>
-  <si>
-    <t>Invisible</t>
-  </si>
-  <si>
-    <t>Armoured</t>
   </si>
   <si>
     <t>Metal</t>
@@ -94,11 +88,32 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
+  <dxfs count="25">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
         </patternFill>
       </fill>
     </dxf>
@@ -112,6 +127,20 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="7"/>
         </patternFill>
       </fill>
@@ -126,20 +155,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="9"/>
         </patternFill>
       </fill>
@@ -147,6 +162,20 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="7"/>
         </patternFill>
       </fill>
@@ -161,20 +190,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="9"/>
         </patternFill>
       </fill>
@@ -182,6 +197,20 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="7"/>
         </patternFill>
       </fill>
@@ -196,7 +225,42 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="3"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
         </patternFill>
       </fill>
     </dxf>
@@ -206,8 +270,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="R2:R7" totalsRowShown="0">
-  <autoFilter ref="R2:R7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="R2:R5" totalsRowShown="0">
+  <autoFilter ref="R2:R5"/>
   <tableColumns count="1">
     <tableColumn id="1" name="Bricks"/>
   </tableColumns>
@@ -503,7 +567,7 @@
   <dimension ref="A1:R32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" customHeight="1"/>
@@ -526,7 +590,7 @@
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="15" customHeight="1">
@@ -547,10 +611,10 @@
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
       <c r="Q2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="R2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="15" customHeight="1">
@@ -571,7 +635,7 @@
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="R3" t="s">
         <v>0</v>
@@ -595,7 +659,7 @@
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
       <c r="Q4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="R4" t="s">
         <v>1</v>
@@ -607,35 +671,35 @@
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
       <c r="Q5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="R5" t="s">
         <v>2</v>
@@ -647,37 +711,34 @@
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
       <c r="Q6" t="s">
-        <v>5</v>
-      </c>
-      <c r="R6" t="s">
         <v>3</v>
       </c>
     </row>
@@ -687,38 +748,35 @@
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
       <c r="Q7" t="s">
-        <v>5</v>
-      </c>
-      <c r="R7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="15" customHeight="1">
@@ -727,35 +785,35 @@
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
       <c r="Q8" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="15" customHeight="1">
@@ -764,35 +822,35 @@
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
       <c r="Q9" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="15" customHeight="1">
@@ -801,35 +859,35 @@
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
       <c r="Q10" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="15" customHeight="1">
@@ -838,35 +896,35 @@
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
       <c r="Q11" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="15" customHeight="1">
@@ -875,35 +933,35 @@
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
       <c r="Q12" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="15" customHeight="1">
@@ -911,20 +969,36 @@
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
+      <c r="E13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
       <c r="Q13" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="15" customHeight="1">
@@ -945,7 +1019,7 @@
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
       <c r="Q14" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="15" customHeight="1">
@@ -966,7 +1040,7 @@
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
       <c r="Q15" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="15" customHeight="1">
@@ -987,7 +1061,7 @@
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
       <c r="Q16" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:17" ht="15" customHeight="1">
@@ -1008,7 +1082,7 @@
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
       <c r="Q17" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:17" ht="15" customHeight="1">
@@ -1029,7 +1103,7 @@
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
       <c r="Q18" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:17" ht="15" customHeight="1">
@@ -1050,7 +1124,7 @@
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
       <c r="Q19" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:17" ht="15" customHeight="1">
@@ -1071,7 +1145,7 @@
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
       <c r="Q20" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:17" ht="15" customHeight="1">
@@ -1092,7 +1166,7 @@
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
       <c r="Q21" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:17" ht="15" customHeight="1">
@@ -1113,7 +1187,7 @@
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
       <c r="Q22" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:17" ht="15" customHeight="1">
@@ -1134,7 +1208,7 @@
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
       <c r="Q23" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:17" ht="15" customHeight="1">
@@ -1155,7 +1229,7 @@
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
       <c r="Q24" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:17" ht="15" customHeight="1">
@@ -1176,7 +1250,7 @@
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
       <c r="Q25" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:17" ht="15" customHeight="1">
@@ -1197,7 +1271,7 @@
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
       <c r="Q26" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:17" ht="15" customHeight="1">
@@ -1218,7 +1292,7 @@
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
       <c r="Q27" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:17" ht="15" customHeight="1">
@@ -1239,7 +1313,7 @@
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
       <c r="Q28" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:17" ht="15" customHeight="1">
@@ -1260,7 +1334,7 @@
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
       <c r="Q29" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:17" ht="15" customHeight="1">
@@ -1281,7 +1355,7 @@
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
       <c r="Q30" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:17" ht="15" customHeight="1">
@@ -1302,7 +1376,7 @@
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
       <c r="Q31" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32" spans="1:17" ht="15" customHeight="1">
@@ -1323,30 +1397,30 @@
       <c r="O32" s="1"/>
       <c r="P32" s="1"/>
       <c r="Q32" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:P32">
-    <cfRule type="cellIs" dxfId="14" priority="11" operator="equal">
-      <formula>$R$7</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="12" operator="equal">
-      <formula>$R$6</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="21" operator="equal">
       <formula>$R$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="22" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="23" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="21" priority="24" operator="equal">
       <formula>$R$4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="25" operator="equal">
       <formula>$R$3</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" sqref="A1:P32">
-      <formula1>$R$3:$R$7</formula1>
+      <formula1>$R$3:$R$5</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fix a collision bug with the paddle and add instructions to start screen
</commit_message>
<xml_diff>
--- a/resources/LevelEditor.xlsx
+++ b/resources/LevelEditor.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="5">
   <si>
     <t>Normal</t>
   </si>
@@ -88,42 +88,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="20">
     <dxf>
       <fill>
         <patternFill>
@@ -567,7 +532,7 @@
   <dimension ref="A1:R32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" customHeight="1"/>
@@ -670,30 +635,14 @@
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
@@ -710,30 +659,14 @@
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
-      <c r="E6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
@@ -747,30 +680,14 @@
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
@@ -784,30 +701,26 @@
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="E8" s="1"/>
       <c r="F8" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>1</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
@@ -819,34 +732,42 @@
     <row r="9" spans="1:18" ht="15" customHeight="1">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+      <c r="C9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="E9" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>1</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>1</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
       <c r="Q9" t="s">
@@ -855,189 +776,309 @@
     </row>
     <row r="10" spans="1:18" ht="15" customHeight="1">
       <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="E10" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>1</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="P10" s="1"/>
       <c r="Q10" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="15" customHeight="1">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
+      <c r="A11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="E11" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>1</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="Q11" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="15" customHeight="1">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
+      <c r="A12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="E12" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>1</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
+      <c r="M12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="Q12" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="15" customHeight="1">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
+      <c r="A13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="E13" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>1</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>1</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
-      <c r="P13" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="Q13" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="15" customHeight="1">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
-      <c r="O14" s="1"/>
-      <c r="P14" s="1"/>
+      <c r="A14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="Q14" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="15" customHeight="1">
       <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
-      <c r="O15" s="1"/>
+      <c r="B15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="P15" s="1"/>
       <c r="Q15" t="s">
         <v>3</v>
@@ -1046,18 +1087,42 @@
     <row r="16" spans="1:18" ht="15" customHeight="1">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
+      <c r="C16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
       <c r="Q16" t="s">
@@ -1070,12 +1135,24 @@
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
+      <c r="F17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
@@ -1401,20 +1478,20 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:P32">
-    <cfRule type="cellIs" dxfId="24" priority="21" operator="equal">
+  <conditionalFormatting sqref="D12:D32 D1:D10 B11:P15 C10:O16 A1:C32 D9:N17 E1:P32">
+    <cfRule type="cellIs" dxfId="19" priority="21" operator="equal">
       <formula>$R$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="22" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="23" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="24" operator="equal">
       <formula>$R$4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="25" operator="equal">
       <formula>$R$3</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>